<commit_message>
IGA design: Use cases and update of reporting.
</commit_message>
<xml_diff>
--- a/midpoint/devel/iga/access-request/access-requests-report-example.xlsx
+++ b/midpoint/devel/iga/access-request/access-requests-report-example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin\gitProjects\docs\midpoint\devel\iga\role-request\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin\gitProjects\docs\midpoint\devel\iga\access-request\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Requests" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requests!$A$3:$Q$25</definedName>
@@ -277,9 +278,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
-    <numFmt numFmtId="166" formatCode="dd/mm/yyyy\ hh:mm"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
-    <numFmt numFmtId="169" formatCode="0.0\ \d"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0\ \d"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -370,20 +371,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -399,15 +388,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,7 +692,7 @@
   <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="Q4" sqref="Q4:Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,89 +719,89 @@
       <c r="A1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="O1" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="P1" s="18">
+      <c r="P1" s="14">
         <v>44622.434027777781</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="4" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="6" t="s">
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="5" t="s">
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="5"/>
-    </row>
-    <row r="3" spans="1:17" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="P2" s="20"/>
+    </row>
+    <row r="3" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="M3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="11" t="s">
+      <c r="N3" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="O3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="P3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="15" t="s">
+      <c r="Q3" s="11" t="s">
         <v>73</v>
       </c>
     </row>
@@ -808,7 +809,7 @@
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="4">
         <v>44617.656631944446</v>
       </c>
       <c r="C4" t="s">
@@ -829,31 +830,31 @@
       <c r="H4">
         <v>2</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="4">
         <v>44617.723993055559</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="8">
+      <c r="K4" s="4">
         <v>44617.726076388892</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
       </c>
-      <c r="M4" s="7">
+      <c r="M4" s="3">
         <v>1</v>
       </c>
-      <c r="N4" s="8">
+      <c r="N4" s="4">
         <v>44620.606446759259</v>
       </c>
       <c r="O4" t="s">
         <v>21</v>
       </c>
-      <c r="P4" s="8">
+      <c r="P4" s="4">
         <v>44620.606446759259</v>
       </c>
-      <c r="Q4" s="16">
+      <c r="Q4" s="12">
         <f>IF(ISBLANK(P4),$P$1,P4)-B4</f>
         <v>2.9498148148122709</v>
       </c>
@@ -862,7 +863,7 @@
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="4">
         <v>44617.661111111112</v>
       </c>
       <c r="C5" t="s">
@@ -883,18 +884,18 @@
       <c r="H5">
         <v>3</v>
       </c>
-      <c r="I5" s="8"/>
+      <c r="I5" s="4"/>
       <c r="J5" t="s">
         <v>57</v>
       </c>
-      <c r="K5" s="8"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="8"/>
+      <c r="K5" s="4"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="4"/>
       <c r="O5" t="s">
         <v>58</v>
       </c>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="16">
+      <c r="P5" s="4"/>
+      <c r="Q5" s="12">
         <f t="shared" ref="Q5:Q25" si="0">IF(ISBLANK(P5),$P$1,P5)-B5</f>
         <v>4.7729166666686069</v>
       </c>
@@ -903,7 +904,7 @@
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="4">
         <v>44617.667048611111</v>
       </c>
       <c r="C6" t="s">
@@ -924,29 +925,29 @@
       <c r="H6">
         <v>3</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="4">
         <v>44620.399305555555</v>
       </c>
       <c r="J6" t="s">
         <v>23</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="4">
         <v>44620.399305555555</v>
       </c>
       <c r="L6" t="s">
         <v>54</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M6" s="3">
         <v>0</v>
       </c>
-      <c r="N6" s="8"/>
+      <c r="N6" s="4"/>
       <c r="O6" t="s">
         <v>21</v>
       </c>
-      <c r="P6" s="8">
+      <c r="P6" s="4">
         <v>44620.399305555555</v>
       </c>
-      <c r="Q6" s="16">
+      <c r="Q6" s="12">
         <f t="shared" si="0"/>
         <v>2.7322569444440887</v>
       </c>
@@ -955,7 +956,7 @@
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="4">
         <v>44617.726076388892</v>
       </c>
       <c r="C7" t="s">
@@ -973,29 +974,29 @@
       <c r="G7" t="s">
         <v>54</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="4">
         <v>44617.726076388892</v>
       </c>
       <c r="J7" t="s">
         <v>23</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7" s="4">
         <v>44617.727465277778</v>
       </c>
       <c r="L7" t="s">
         <v>54</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="3">
         <v>0</v>
       </c>
-      <c r="N7" s="8"/>
+      <c r="N7" s="4"/>
       <c r="O7" t="s">
         <v>21</v>
       </c>
-      <c r="P7" s="8">
+      <c r="P7" s="4">
         <v>44617.727465277778</v>
       </c>
-      <c r="Q7" s="16">
+      <c r="Q7" s="12">
         <f t="shared" si="0"/>
         <v>1.3888888861401938E-3</v>
       </c>
@@ -1004,7 +1005,7 @@
       <c r="A8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="4">
         <v>44620.334027777775</v>
       </c>
       <c r="C8" t="s">
@@ -1022,27 +1023,27 @@
       <c r="G8" t="s">
         <v>60</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="4">
         <v>44620.416666666664</v>
       </c>
       <c r="J8" t="s">
         <v>54</v>
       </c>
-      <c r="K8" s="8"/>
+      <c r="K8" s="4"/>
       <c r="L8" t="s">
         <v>54</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="3">
         <v>0</v>
       </c>
-      <c r="N8" s="8"/>
+      <c r="N8" s="4"/>
       <c r="O8" t="s">
         <v>60</v>
       </c>
-      <c r="P8" s="8">
+      <c r="P8" s="4">
         <v>44620.416666666664</v>
       </c>
-      <c r="Q8" s="16">
+      <c r="Q8" s="12">
         <f t="shared" si="0"/>
         <v>8.2638888889050577E-2</v>
       </c>
@@ -1051,7 +1052,7 @@
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="4">
         <v>44620.340312499997</v>
       </c>
       <c r="C9" t="s">
@@ -1072,31 +1073,31 @@
       <c r="H9">
         <v>1</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="4">
         <v>44621.427118055559</v>
       </c>
       <c r="J9" t="s">
         <v>23</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9" s="4">
         <v>44621.427719907406</v>
       </c>
       <c r="L9" t="s">
         <v>23</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M9" s="3">
         <v>2</v>
       </c>
-      <c r="N9" s="8">
+      <c r="N9" s="4">
         <v>44623.605937499997</v>
       </c>
       <c r="O9" t="s">
         <v>21</v>
       </c>
-      <c r="P9" s="8">
+      <c r="P9" s="4">
         <v>44623.605937499997</v>
       </c>
-      <c r="Q9" s="16">
+      <c r="Q9" s="12">
         <f t="shared" si="0"/>
         <v>3.265625</v>
       </c>
@@ -1105,7 +1106,7 @@
       <c r="A10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="4">
         <v>44620.34170138889</v>
       </c>
       <c r="C10" t="s">
@@ -1126,31 +1127,31 @@
       <c r="H10">
         <v>1</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="4">
         <v>44621.427118055559</v>
       </c>
       <c r="J10" t="s">
         <v>23</v>
       </c>
-      <c r="K10" s="8">
+      <c r="K10" s="4">
         <v>44621.427719907406</v>
       </c>
       <c r="L10" t="s">
         <v>23</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M10" s="3">
         <v>2</v>
       </c>
-      <c r="N10" s="8">
+      <c r="N10" s="4">
         <v>44623.608020833337</v>
       </c>
       <c r="O10" t="s">
         <v>21</v>
       </c>
-      <c r="P10" s="8">
+      <c r="P10" s="4">
         <v>44623.608020833337</v>
       </c>
-      <c r="Q10" s="16">
+      <c r="Q10" s="12">
         <f t="shared" si="0"/>
         <v>3.2663194444467081</v>
       </c>
@@ -1159,7 +1160,7 @@
       <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="4">
         <v>44620.342395833337</v>
       </c>
       <c r="C11" t="s">
@@ -1180,31 +1181,31 @@
       <c r="H11">
         <v>1</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="4">
         <v>44621.427118055559</v>
       </c>
       <c r="J11" t="s">
         <v>23</v>
       </c>
-      <c r="K11" s="8">
+      <c r="K11" s="4">
         <v>44621.427719907406</v>
       </c>
       <c r="L11" t="s">
         <v>23</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M11" s="3">
         <v>2</v>
       </c>
-      <c r="N11" s="8">
+      <c r="N11" s="4">
         <v>44623.61010416667</v>
       </c>
       <c r="O11" t="s">
         <v>21</v>
       </c>
-      <c r="P11" s="8">
+      <c r="P11" s="4">
         <v>44623.61010416667</v>
       </c>
-      <c r="Q11" s="16">
+      <c r="Q11" s="12">
         <f t="shared" si="0"/>
         <v>3.2677083333328483</v>
       </c>
@@ -1213,7 +1214,7 @@
       <c r="A12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="4">
         <v>44620.343090277776</v>
       </c>
       <c r="C12" t="s">
@@ -1234,31 +1235,31 @@
       <c r="H12">
         <v>1</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="4">
         <v>44621.427118055559</v>
       </c>
       <c r="J12" t="s">
         <v>23</v>
       </c>
-      <c r="K12" s="8">
+      <c r="K12" s="4">
         <v>44621.427719907406</v>
       </c>
-      <c r="L12" s="19" t="s">
+      <c r="L12" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="3">
         <v>2</v>
       </c>
-      <c r="N12" s="8">
+      <c r="N12" s="4">
         <v>44623.611493055556</v>
       </c>
-      <c r="O12" s="19" t="s">
+      <c r="O12" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="P12" s="8">
+      <c r="P12" s="4">
         <v>44623.611493055556</v>
       </c>
-      <c r="Q12" s="16">
+      <c r="Q12" s="12">
         <f t="shared" si="0"/>
         <v>3.2684027777795563</v>
       </c>
@@ -1267,7 +1268,7 @@
       <c r="A13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="4">
         <v>44620.371527777781</v>
       </c>
       <c r="C13" t="s">
@@ -1288,29 +1289,29 @@
       <c r="H13">
         <v>1</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="4">
         <v>44620.384027777778</v>
       </c>
       <c r="J13" t="s">
         <v>23</v>
       </c>
-      <c r="K13" s="8">
+      <c r="K13" s="4">
         <v>44620.384027777778</v>
       </c>
       <c r="L13" t="s">
         <v>54</v>
       </c>
-      <c r="M13" s="7">
+      <c r="M13" s="3">
         <v>0</v>
       </c>
-      <c r="N13" s="8"/>
+      <c r="N13" s="4"/>
       <c r="O13" t="s">
         <v>21</v>
       </c>
-      <c r="P13" s="8">
+      <c r="P13" s="4">
         <v>44620.384027777778</v>
       </c>
-      <c r="Q13" s="16">
+      <c r="Q13" s="12">
         <f t="shared" si="0"/>
         <v>1.2499999997089617E-2</v>
       </c>
@@ -1319,7 +1320,7 @@
       <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="4">
         <v>44620.374305555553</v>
       </c>
       <c r="C14" t="s">
@@ -1340,29 +1341,29 @@
       <c r="H14">
         <v>2</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="4">
         <v>44620.500694444447</v>
       </c>
       <c r="J14" t="s">
         <v>23</v>
       </c>
-      <c r="K14" s="8">
+      <c r="K14" s="4">
         <v>44620.500694444447</v>
       </c>
       <c r="L14" t="s">
         <v>54</v>
       </c>
-      <c r="M14" s="7">
+      <c r="M14" s="3">
         <v>0</v>
       </c>
-      <c r="N14" s="8"/>
+      <c r="N14" s="4"/>
       <c r="O14" t="s">
         <v>21</v>
       </c>
-      <c r="P14" s="8">
+      <c r="P14" s="4">
         <v>44620.500694444447</v>
       </c>
-      <c r="Q14" s="16">
+      <c r="Q14" s="12">
         <f t="shared" si="0"/>
         <v>0.12638888889341615</v>
       </c>
@@ -1371,7 +1372,7 @@
       <c r="A15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="4">
         <v>44620.384756944448</v>
       </c>
       <c r="C15" t="s">
@@ -1392,29 +1393,29 @@
       <c r="H15">
         <v>2</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="4">
         <v>44620.500694444447</v>
       </c>
       <c r="J15" t="s">
         <v>23</v>
       </c>
-      <c r="K15" s="8">
+      <c r="K15" s="4">
         <v>44620.500694444447</v>
       </c>
       <c r="L15" t="s">
         <v>54</v>
       </c>
-      <c r="M15" s="7">
+      <c r="M15" s="3">
         <v>0</v>
       </c>
-      <c r="N15" s="8"/>
+      <c r="N15" s="4"/>
       <c r="O15" t="s">
         <v>21</v>
       </c>
-      <c r="P15" s="8">
+      <c r="P15" s="4">
         <v>44620.500694444447</v>
       </c>
-      <c r="Q15" s="16">
+      <c r="Q15" s="12">
         <f t="shared" si="0"/>
         <v>0.11593749999883585</v>
       </c>
@@ -1423,7 +1424,7 @@
       <c r="A16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="4">
         <v>44620.397951388892</v>
       </c>
       <c r="C16" t="s">
@@ -1444,29 +1445,29 @@
       <c r="H16">
         <v>1</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I16" s="4">
         <v>44620.621527777781</v>
       </c>
       <c r="J16" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="8">
+      <c r="K16" s="4">
         <v>44620.622916666667</v>
       </c>
       <c r="L16" t="s">
         <v>54</v>
       </c>
-      <c r="M16" s="7">
+      <c r="M16" s="3">
         <v>0</v>
       </c>
-      <c r="N16" s="8"/>
+      <c r="N16" s="4"/>
       <c r="O16" t="s">
         <v>21</v>
       </c>
-      <c r="P16" s="8">
+      <c r="P16" s="4">
         <v>44620.622916666667</v>
       </c>
-      <c r="Q16" s="16">
+      <c r="Q16" s="12">
         <f t="shared" si="0"/>
         <v>0.22496527777548181</v>
       </c>
@@ -1475,7 +1476,7 @@
       <c r="A17" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="4">
         <v>44620.406284722223</v>
       </c>
       <c r="C17" t="s">
@@ -1496,29 +1497,29 @@
       <c r="H17">
         <v>3</v>
       </c>
-      <c r="I17" s="8">
+      <c r="I17" s="4">
         <v>44621.34375</v>
       </c>
       <c r="J17" t="s">
         <v>23</v>
       </c>
-      <c r="K17" s="8">
+      <c r="K17" s="4">
         <v>44621.34375</v>
       </c>
       <c r="L17" t="s">
         <v>54</v>
       </c>
-      <c r="M17" s="7">
+      <c r="M17" s="3">
         <v>0</v>
       </c>
-      <c r="N17" s="8"/>
+      <c r="N17" s="4"/>
       <c r="O17" t="s">
         <v>21</v>
       </c>
-      <c r="P17" s="8">
+      <c r="P17" s="4">
         <v>44621.34375</v>
       </c>
-      <c r="Q17" s="16">
+      <c r="Q17" s="12">
         <f t="shared" si="0"/>
         <v>0.937465277776937</v>
       </c>
@@ -1527,7 +1528,7 @@
       <c r="A18" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="4">
         <v>44620.416666666664</v>
       </c>
       <c r="C18" t="s">
@@ -1548,27 +1549,27 @@
       <c r="H18">
         <v>2</v>
       </c>
-      <c r="I18" s="8">
+      <c r="I18" s="4">
         <v>44620.690972222219</v>
       </c>
       <c r="J18" t="s">
         <v>54</v>
       </c>
-      <c r="K18" s="8"/>
+      <c r="K18" s="4"/>
       <c r="L18" t="s">
         <v>54</v>
       </c>
-      <c r="M18" s="7">
+      <c r="M18" s="3">
         <v>0</v>
       </c>
-      <c r="N18" s="8"/>
+      <c r="N18" s="4"/>
       <c r="O18" t="s">
         <v>60</v>
       </c>
-      <c r="P18" s="8">
+      <c r="P18" s="4">
         <v>44620.690972222219</v>
       </c>
-      <c r="Q18" s="16">
+      <c r="Q18" s="12">
         <f t="shared" si="0"/>
         <v>0.27430555555474712</v>
       </c>
@@ -1577,7 +1578,7 @@
       <c r="A19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="4">
         <v>44620.425000000003</v>
       </c>
       <c r="C19" t="s">
@@ -1598,29 +1599,29 @@
       <c r="H19">
         <v>1</v>
       </c>
-      <c r="I19" s="8">
+      <c r="I19" s="4">
         <v>44621.482638888891</v>
       </c>
-      <c r="J19" s="19" t="s">
+      <c r="J19" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="K19" s="8">
+      <c r="K19" s="4">
         <v>44621.5</v>
       </c>
       <c r="L19" t="s">
         <v>54</v>
       </c>
-      <c r="M19" s="7">
+      <c r="M19" s="3">
         <v>0</v>
       </c>
-      <c r="N19" s="8"/>
-      <c r="O19" s="19" t="s">
+      <c r="N19" s="4"/>
+      <c r="O19" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="P19" s="8">
+      <c r="P19" s="4">
         <v>44621.5</v>
       </c>
-      <c r="Q19" s="16">
+      <c r="Q19" s="12">
         <f t="shared" si="0"/>
         <v>1.0749999999970896</v>
       </c>
@@ -1629,7 +1630,7 @@
       <c r="A20" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="4">
         <v>44620.425694444442</v>
       </c>
       <c r="C20" t="s">
@@ -1650,29 +1651,29 @@
       <c r="H20">
         <v>1</v>
       </c>
-      <c r="I20" s="8">
+      <c r="I20" s="4">
         <v>44621.482638888891</v>
       </c>
-      <c r="J20" s="19" t="s">
+      <c r="J20" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="K20" s="8">
+      <c r="K20" s="4">
         <v>44621.5</v>
       </c>
       <c r="L20" t="s">
         <v>54</v>
       </c>
-      <c r="M20" s="7">
+      <c r="M20" s="3">
         <v>0</v>
       </c>
-      <c r="N20" s="8"/>
-      <c r="O20" s="19" t="s">
+      <c r="N20" s="4"/>
+      <c r="O20" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="P20" s="8">
+      <c r="P20" s="4">
         <v>44621.5</v>
       </c>
-      <c r="Q20" s="16">
+      <c r="Q20" s="12">
         <f t="shared" si="0"/>
         <v>1.0743055555576575</v>
       </c>
@@ -1681,7 +1682,7 @@
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="4">
         <v>44620.426388888889</v>
       </c>
       <c r="C21" t="s">
@@ -1702,29 +1703,29 @@
       <c r="H21">
         <v>1</v>
       </c>
-      <c r="I21" s="8">
+      <c r="I21" s="4">
         <v>44621.482638888891</v>
       </c>
-      <c r="J21" s="19" t="s">
+      <c r="J21" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="K21" s="8">
+      <c r="K21" s="4">
         <v>44621.5</v>
       </c>
       <c r="L21" t="s">
         <v>54</v>
       </c>
-      <c r="M21" s="7">
+      <c r="M21" s="3">
         <v>0</v>
       </c>
-      <c r="N21" s="8"/>
-      <c r="O21" s="19" t="s">
+      <c r="N21" s="4"/>
+      <c r="O21" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="P21" s="8">
+      <c r="P21" s="4">
         <v>44621.5</v>
       </c>
-      <c r="Q21" s="16">
+      <c r="Q21" s="12">
         <f t="shared" si="0"/>
         <v>1.0736111111109494</v>
       </c>
@@ -1733,7 +1734,7 @@
       <c r="A22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22" s="4">
         <v>44620.524305555555</v>
       </c>
       <c r="C22" t="s">
@@ -1754,18 +1755,18 @@
       <c r="H22">
         <v>1</v>
       </c>
-      <c r="I22" s="8"/>
-      <c r="J22" s="20" t="s">
+      <c r="I22" s="4"/>
+      <c r="J22" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="K22" s="8"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="8"/>
+      <c r="K22" s="4"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="4"/>
       <c r="O22" t="s">
         <v>58</v>
       </c>
-      <c r="P22" s="8"/>
-      <c r="Q22" s="16">
+      <c r="P22" s="4"/>
+      <c r="Q22" s="12">
         <f t="shared" si="0"/>
         <v>1.9097222222262644</v>
       </c>
@@ -1774,7 +1775,7 @@
       <c r="A23" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23" s="4">
         <v>44620.677083333336</v>
       </c>
       <c r="C23" t="s">
@@ -1795,29 +1796,29 @@
       <c r="H23">
         <v>2</v>
       </c>
-      <c r="I23" s="8">
+      <c r="I23" s="4">
         <v>44622.350694444445</v>
       </c>
       <c r="J23" t="s">
         <v>23</v>
       </c>
-      <c r="K23" s="8">
+      <c r="K23" s="4">
         <v>44622.352083333331</v>
       </c>
       <c r="L23" t="s">
         <v>54</v>
       </c>
-      <c r="M23" s="7">
+      <c r="M23" s="3">
         <v>0</v>
       </c>
-      <c r="N23" s="8"/>
+      <c r="N23" s="4"/>
       <c r="O23" t="s">
         <v>21</v>
       </c>
-      <c r="P23" s="8">
+      <c r="P23" s="4">
         <v>44622.352083333331</v>
       </c>
-      <c r="Q23" s="16">
+      <c r="Q23" s="12">
         <f t="shared" si="0"/>
         <v>1.6749999999956344</v>
       </c>
@@ -1826,7 +1827,7 @@
       <c r="A24" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24" s="4">
         <v>44620.678472222222</v>
       </c>
       <c r="C24" t="s">
@@ -1847,29 +1848,29 @@
       <c r="H24">
         <v>2</v>
       </c>
-      <c r="I24" s="8">
+      <c r="I24" s="4">
         <v>44622.350694444445</v>
       </c>
       <c r="J24" t="s">
         <v>23</v>
       </c>
-      <c r="K24" s="8">
+      <c r="K24" s="4">
         <v>44622.352083333331</v>
       </c>
       <c r="L24" t="s">
         <v>54</v>
       </c>
-      <c r="M24" s="7">
+      <c r="M24" s="3">
         <v>0</v>
       </c>
-      <c r="N24" s="8"/>
+      <c r="N24" s="4"/>
       <c r="O24" t="s">
         <v>21</v>
       </c>
-      <c r="P24" s="8">
+      <c r="P24" s="4">
         <v>44622.352083333331</v>
       </c>
-      <c r="Q24" s="16">
+      <c r="Q24" s="12">
         <f t="shared" si="0"/>
         <v>1.6736111111094942</v>
       </c>
@@ -1878,7 +1879,7 @@
       <c r="A25" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B25" s="4">
         <v>44620.684027777781</v>
       </c>
       <c r="C25" t="s">
@@ -1899,46 +1900,46 @@
       <c r="H25">
         <v>2</v>
       </c>
-      <c r="I25" s="8">
+      <c r="I25" s="4">
         <v>44622.350694444445</v>
       </c>
       <c r="J25" t="s">
         <v>23</v>
       </c>
-      <c r="K25" s="8">
+      <c r="K25" s="4">
         <v>44622.352083333331</v>
       </c>
       <c r="L25" t="s">
         <v>54</v>
       </c>
-      <c r="M25" s="7">
+      <c r="M25" s="3">
         <v>0</v>
       </c>
-      <c r="N25" s="8"/>
+      <c r="N25" s="4"/>
       <c r="O25" t="s">
         <v>21</v>
       </c>
-      <c r="P25" s="8">
+      <c r="P25" s="4">
         <v>44622.352083333331</v>
       </c>
-      <c r="Q25" s="16">
+      <c r="Q25" s="12">
         <f t="shared" si="0"/>
         <v>1.6680555555503815</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
-      <c r="B26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="8"/>
-      <c r="P26" s="8"/>
-      <c r="Q26" s="14"/>
+      <c r="B26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="10"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="I27" s="8"/>
-      <c r="Q27" s="14"/>
+      <c r="I27" s="4"/>
+      <c r="Q27" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="A3:Q25"/>
@@ -1951,4 +1952,88 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12"/>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="12"/>
+    </row>
+  </sheetData>
+  <sortState ref="A1:A22">
+    <sortCondition ref="A1:A22"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>